<commit_message>
revision de auditoria cierre multiples proyectos
</commit_message>
<xml_diff>
--- a/Proyectos/2015/12/P1383 - RNCFAC, Juan Lopez _ MO/Calidad/No_conformidades.xlsx
+++ b/Proyectos/2015/12/P1383 - RNCFAC, Juan Lopez _ MO/Calidad/No_conformidades.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>REPORTE DE NO CONFORMIDADES P1383 - RNCFAC, Juan Lopez _ MO</t>
   </si>
@@ -47,16 +47,13 @@
     <t>Marisol Ornelas</t>
   </si>
   <si>
-    <t>En proceso</t>
+    <t>Cerrada</t>
   </si>
   <si>
     <t>hablar en la próxima minuta sobre el proyecto</t>
   </si>
   <si>
     <t>Nohay evidencia del proceso de cierre</t>
-  </si>
-  <si>
-    <t>Cerrada</t>
   </si>
   <si>
     <t>crear la actividad de cierre como responsable asignar a judith quien genera la encuesta de satisfacción para generar el cierre de proyecto, enviar la carta de aceptación por correo y dejar evidencia</t>
@@ -328,7 +325,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -400,7 +397,9 @@
       <c r="D4" s="5" t="n">
         <v>42382</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5" t="n">
+        <v>42387</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
@@ -425,10 +424,10 @@
         <v>42383</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,7 +435,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
@@ -448,10 +447,10 @@
         <v>42383</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,7 +458,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
@@ -471,10 +470,10 @@
         <v>42383</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,7 +481,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
@@ -494,10 +493,10 @@
         <v>42383</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,7 +504,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>9</v>
@@ -517,10 +516,10 @@
         <v>42383</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>